<commit_message>
UpDate: Genere una nueva estadistica
</commit_message>
<xml_diff>
--- a/model_evaluations.xlsx
+++ b/model_evaluations.xlsx
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.1680486291988199</v>
+        <v>0.008385555716303728</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.000121552497059696</v>
+        <v>0.07495212848405852</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
UpDate: Nuevo Archivo para funcionamiento Dash
</commit_message>
<xml_diff>
--- a/model_evaluations.xlsx
+++ b/model_evaluations.xlsx
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.008385555716303728</v>
+        <v>0.146658249084617</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.07495212848405852</v>
+        <v>0.1791277310152607</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>

</xml_diff>